<commit_message>
modified excel file -> test was successful!
</commit_message>
<xml_diff>
--- a/нейр.xlsx
+++ b/нейр.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmo083\Dropbox\PythonProject\Code\Daulet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Нейрохирургия" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="57">
   <si>
     <t>МО</t>
   </si>
@@ -525,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,9 +638,6 @@
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
       <c r="B2">
         <v>172</v>
       </c>
@@ -1038,6 +1035,410 @@
         <v>48</v>
       </c>
       <c r="AG5">
+        <v>5697067.9342231303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>172</v>
+      </c>
+      <c r="C7">
+        <v>7193907</v>
+      </c>
+      <c r="D7">
+        <v>395390817</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>133450</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7">
+        <v>53</v>
+      </c>
+      <c r="S7">
+        <v>12</v>
+      </c>
+      <c r="T7" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD7">
+        <v>11.0067</v>
+      </c>
+      <c r="AE7">
+        <v>5032</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG7">
+        <v>5697067.9342231303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>172</v>
+      </c>
+      <c r="C8">
+        <v>7193907</v>
+      </c>
+      <c r="D8">
+        <v>395390817</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8">
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <v>133450</v>
+      </c>
+      <c r="J8">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8">
+        <v>53</v>
+      </c>
+      <c r="S8">
+        <v>12</v>
+      </c>
+      <c r="T8" t="s">
+        <v>50</v>
+      </c>
+      <c r="U8" t="s">
+        <v>51</v>
+      </c>
+      <c r="V8" t="s">
+        <v>41</v>
+      </c>
+      <c r="W8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y8">
+        <v>3</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8">
+        <v>11.0067</v>
+      </c>
+      <c r="AE8">
+        <v>5032</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG8">
+        <v>5697067.9342231303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>172</v>
+      </c>
+      <c r="C9">
+        <v>7193907</v>
+      </c>
+      <c r="D9">
+        <v>395390817</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>133450</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9">
+        <v>53</v>
+      </c>
+      <c r="S9">
+        <v>12</v>
+      </c>
+      <c r="T9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" t="s">
+        <v>51</v>
+      </c>
+      <c r="V9" t="s">
+        <v>41</v>
+      </c>
+      <c r="W9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y9">
+        <v>3</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD9">
+        <v>11.0067</v>
+      </c>
+      <c r="AE9">
+        <v>5032</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG9">
+        <v>5697067.9342231303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>172</v>
+      </c>
+      <c r="C10">
+        <v>7193907</v>
+      </c>
+      <c r="D10">
+        <v>395390817</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>133450</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10">
+        <v>53</v>
+      </c>
+      <c r="S10">
+        <v>12</v>
+      </c>
+      <c r="T10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10" t="s">
+        <v>51</v>
+      </c>
+      <c r="V10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10">
+        <v>3</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD10">
+        <v>11.0067</v>
+      </c>
+      <c r="AE10">
+        <v>5032</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG10">
         <v>5697067.9342231303</v>
       </c>
     </row>

</xml_diff>